<commit_message>
Final changes to structure
</commit_message>
<xml_diff>
--- a/Postep.xlsx
+++ b/Postep.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasoh\Documents\STUDIA\HACKATHON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EFA3B5-639F-414F-95B3-F96BF1FBF19C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C01093D-E094-406E-AA6D-12CB24D0CD02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{54F5C51C-4280-46D3-B986-549A3B50E979}"/>
+    <workbookView xWindow="16020" yWindow="3345" windowWidth="21600" windowHeight="11385" xr2:uid="{54F5C51C-4280-46D3-B986-549A3B50E979}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -673,8 +673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D5CABF-4E77-4560-BB05-FDD6091D2B2A}">
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +861,7 @@
       <c r="I5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="J5" s="1" t="s">
         <v>58</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -905,7 +905,7 @@
       <c r="K6" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
       </c>
       <c r="P10">
         <f>10 + SUM(B9:L13)</f>
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1029,7 +1029,9 @@
       <c r="I11" s="5">
         <v>1</v>
       </c>
-      <c r="J11" s="5"/>
+      <c r="J11" s="5">
+        <v>1</v>
+      </c>
       <c r="K11" s="5">
         <v>1</v>
       </c>
@@ -1059,7 +1061,9 @@
       <c r="K12" s="5">
         <v>1</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:16" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13">

</xml_diff>